<commit_message>
se mejoro el codigo
</commit_message>
<xml_diff>
--- a/uploads/fichas.xlsx
+++ b/uploads/fichas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AVA\serverbienestar\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{438D6C1E-C09D-40E8-939E-1307C4A3A0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAECAD5E-31CE-429B-B7A3-E5406F87DCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E8933C4E-2A7E-44E3-835E-E34B5A4B41BA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Ficha</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Mercadeo</t>
+  </si>
+  <si>
+    <t>Especialidad</t>
+  </si>
+  <si>
+    <t>lgtc</t>
+  </si>
+  <si>
+    <t>adso</t>
+  </si>
+  <si>
+    <t>adsi</t>
   </si>
 </sst>
 </file>
@@ -80,27 +92,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -109,8 +106,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -447,48 +444,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DEEB133-F945-4D48-8D54-7C7B1AA301B3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>2546847</v>
+        <v>6565414</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2154645</v>
+        <v>5441655</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>9564547</v>
+        <v>3325232</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>